<commit_message>
performed averaging on data
</commit_message>
<xml_diff>
--- a/src/simulation/testing_logs/combined/combined_data.xlsx
+++ b/src/simulation/testing_logs/combined/combined_data.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrwnh/Development/autonomous-navigation/src/simulation/testing_logs/combined/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9F89E113-41C2-B442-B33A-3E86E707C680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{88FD6D04-ECDF-8848-BC0F-0E401334341A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="combined_data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="19">
   <si>
     <t>algo</t>
   </si>
@@ -72,6 +71,12 @@
   </si>
   <si>
     <t>random_walk</t>
+  </si>
+  <si>
+    <t>avg_speed</t>
+  </si>
+  <si>
+    <t>avg_time_taken</t>
   </si>
 </sst>
 </file>
@@ -932,15 +937,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -971,8 +979,14 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1005,8 +1019,14 @@
         <f>250-(I2+H2)</f>
         <v>218</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>81.34</v>
+      </c>
+      <c r="L2">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1039,8 +1059,14 @@
         <f t="shared" ref="J3:J37" si="1">250-(I3+H3)</f>
         <v>216</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>82.62</v>
+      </c>
+      <c r="L3">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1073,8 +1099,14 @@
         <f t="shared" si="1"/>
         <v>213</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>108.25</v>
+      </c>
+      <c r="L4">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1107,8 +1139,14 @@
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>80.97</v>
+      </c>
+      <c r="L5">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1141,8 +1179,14 @@
         <f t="shared" si="1"/>
         <v>197</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>97.5</v>
+      </c>
+      <c r="L6">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1175,8 +1219,14 @@
         <f t="shared" si="1"/>
         <v>186</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>82.24</v>
+      </c>
+      <c r="L7">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1209,8 +1259,14 @@
         <f t="shared" si="1"/>
         <v>182</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>113.68</v>
+      </c>
+      <c r="L8">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1243,8 +1299,14 @@
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>39.26</v>
+      </c>
+      <c r="L9">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1277,8 +1339,14 @@
         <f t="shared" si="1"/>
         <v>184</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>60.01</v>
+      </c>
+      <c r="L10">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1311,8 +1379,14 @@
         <f t="shared" si="1"/>
         <v>185</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>69.77</v>
+      </c>
+      <c r="L11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1345,8 +1419,14 @@
         <f t="shared" si="1"/>
         <v>175</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>124.03</v>
+      </c>
+      <c r="L12">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1379,8 +1459,14 @@
         <f t="shared" si="1"/>
         <v>157</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>15.23</v>
+      </c>
+      <c r="L13">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1413,8 +1499,14 @@
         <f t="shared" si="1"/>
         <v>194</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>69.88</v>
+      </c>
+      <c r="L14">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1447,8 +1539,14 @@
         <f t="shared" si="1"/>
         <v>238</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>65.650000000000006</v>
+      </c>
+      <c r="L15">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1481,8 +1579,14 @@
         <f t="shared" si="1"/>
         <v>239</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>40.74</v>
+      </c>
+      <c r="L16">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1515,8 +1619,14 @@
         <f t="shared" si="1"/>
         <v>238</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>71.91</v>
+      </c>
+      <c r="L17">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1549,8 +1659,14 @@
         <f t="shared" si="1"/>
         <v>137</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <v>77.510000000000005</v>
+      </c>
+      <c r="L18">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1583,8 +1699,14 @@
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>60.77</v>
+      </c>
+      <c r="L19">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1617,8 +1739,14 @@
         <f t="shared" si="1"/>
         <v>208</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>30.68</v>
+      </c>
+      <c r="L20">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1651,8 +1779,14 @@
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>74.88</v>
+      </c>
+      <c r="L21">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1685,8 +1819,14 @@
         <f t="shared" si="1"/>
         <v>138</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <v>72.64</v>
+      </c>
+      <c r="L22">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1719,8 +1859,14 @@
         <f t="shared" si="1"/>
         <v>153</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>87.83</v>
+      </c>
+      <c r="L23">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1753,8 +1899,14 @@
         <f t="shared" si="1"/>
         <v>149</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>50.57</v>
+      </c>
+      <c r="L24">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1787,8 +1939,14 @@
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>104.43</v>
+      </c>
+      <c r="L25">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1821,8 +1979,14 @@
         <f t="shared" si="1"/>
         <v>175</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>91.09</v>
+      </c>
+      <c r="L26">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1855,8 +2019,14 @@
         <f t="shared" si="1"/>
         <v>247</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <v>80.06</v>
+      </c>
+      <c r="L27">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1889,8 +2059,14 @@
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <v>91.94</v>
+      </c>
+      <c r="L28">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1923,8 +2099,14 @@
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1957,8 +2139,14 @@
         <f t="shared" si="1"/>
         <v>193</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30">
+        <v>83.6</v>
+      </c>
+      <c r="L30">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1991,8 +2179,14 @@
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31">
+        <v>56.86</v>
+      </c>
+      <c r="L31">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -2025,8 +2219,14 @@
         <f t="shared" si="1"/>
         <v>226</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <v>59.26</v>
+      </c>
+      <c r="L32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -2059,8 +2259,14 @@
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -2093,8 +2299,14 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34">
+        <v>86.78</v>
+      </c>
+      <c r="L34">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -2127,8 +2339,14 @@
         <f t="shared" si="1"/>
         <v>143</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>84.94</v>
+      </c>
+      <c r="L35">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -2161,8 +2379,14 @@
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>48.68</v>
+      </c>
+      <c r="L36">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -2199,16 +2423,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>